<commit_message>
final changes with comments
</commit_message>
<xml_diff>
--- a/A1/Performance of astar.xlsx
+++ b/A1/Performance of astar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Somesh\PycharmProjects\8_puzzle\AI-algo-code-master\A1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Somesh\PycharmProjects\AI-algo-code\A1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,8 +18,8 @@
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Depth</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>(All)</t>
+  </si>
+  <si>
+    <t>A* Algorithm</t>
+  </si>
+  <si>
+    <t>IDA* Algorithm</t>
   </si>
 </sst>
 </file>
@@ -223,9 +229,6 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -239,6 +242,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -260,7 +266,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Somesh Gupta" refreshedDate="42651.905703009259" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="21">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B2:G23" sheet="Sheet1"/>
+    <worksheetSource ref="B3:G31" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Number of state explored " numFmtId="0">
@@ -297,7 +303,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Somesh Gupta" refreshedDate="42651.906660300927" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="22">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B2:G24" sheet="Sheet1"/>
+    <worksheetSource ref="B3:G32" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Number of state explored " numFmtId="0">
@@ -682,7 +688,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -749,7 +755,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -1081,7 +1087,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
@@ -1089,7 +1095,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
@@ -1106,36 +1112,36 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>4526</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>350216</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>10262</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>59838</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>4526</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>350216</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>10262</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>59838</v>
       </c>
     </row>
@@ -1155,94 +1161,94 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1251,11 +1257,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1263,404 +1267,838 @@
     <col min="2" max="2" width="30.54296875" customWidth="1"/>
     <col min="3" max="3" width="27.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="I1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="I2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>21</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>177</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>36</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>11</v>
+      </c>
+      <c r="L5">
+        <v>185</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>27</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>12</v>
+      </c>
+      <c r="L6">
+        <v>134</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>67</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>22</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <v>7</v>
+      </c>
+      <c r="N7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>31</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>12</v>
+      </c>
+      <c r="L8">
+        <v>44</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>145</v>
+      </c>
+      <c r="F9">
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="I9">
+        <v>86</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>15</v>
+      </c>
+      <c r="L9">
+        <v>1818</v>
+      </c>
+      <c r="M9">
+        <v>17</v>
+      </c>
+      <c r="N9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>132</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="I10">
+        <v>35</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>15</v>
+      </c>
+      <c r="L10">
+        <v>2284</v>
+      </c>
+      <c r="M10">
+        <v>47</v>
+      </c>
+      <c r="N10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>47</v>
+      </c>
+      <c r="B11">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>1652</v>
+      </c>
+      <c r="F11">
+        <v>742</v>
+      </c>
+      <c r="G11">
+        <v>19</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>19</v>
+      </c>
+      <c r="L11">
+        <v>123401</v>
+      </c>
+      <c r="M11">
+        <v>142</v>
+      </c>
+      <c r="N11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>49</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>898</v>
+      </c>
+      <c r="F12">
+        <v>238</v>
+      </c>
+      <c r="G12">
+        <v>18</v>
+      </c>
+      <c r="I12">
+        <v>79</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <v>18</v>
+      </c>
+      <c r="L12">
+        <v>41074</v>
+      </c>
+      <c r="M12">
+        <v>369</v>
+      </c>
+      <c r="N12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>53</v>
+      </c>
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>66</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <v>317</v>
+      </c>
+      <c r="J13">
+        <v>6</v>
+      </c>
+      <c r="K13">
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <v>3274</v>
+      </c>
+      <c r="M13">
+        <v>29</v>
+      </c>
+      <c r="N13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>55</v>
+      </c>
+      <c r="B14">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>21</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>9</v>
+      </c>
+      <c r="I14">
+        <v>30</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>9</v>
+      </c>
+      <c r="L14">
+        <v>138</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>68</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <v>234</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>12</v>
+      </c>
+      <c r="L15">
+        <v>868</v>
+      </c>
+      <c r="M15">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="N15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>65</v>
+      </c>
+      <c r="B16">
+        <v>75</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>395</v>
+      </c>
+      <c r="F16">
+        <v>70</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="I16">
+        <v>610</v>
+      </c>
+      <c r="J16">
+        <v>12</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
+      </c>
+      <c r="L16">
+        <v>18940</v>
+      </c>
+      <c r="M16">
+        <v>163</v>
+      </c>
+      <c r="N16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <v>335</v>
+      </c>
+      <c r="F17">
+        <v>51</v>
+      </c>
+      <c r="G17">
+        <v>18</v>
+      </c>
+      <c r="I17">
+        <v>209</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>18</v>
+      </c>
+      <c r="L17">
+        <v>6344</v>
+      </c>
+      <c r="M17">
+        <v>58</v>
+      </c>
+      <c r="N17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>75</v>
+      </c>
+      <c r="B18">
+        <v>249</v>
+      </c>
+      <c r="C18">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>21</v>
+      </c>
+      <c r="E18">
+        <v>5507</v>
+      </c>
+      <c r="F18">
+        <v>235</v>
+      </c>
+      <c r="G18">
+        <v>21</v>
+      </c>
+      <c r="I18">
+        <v>6496</v>
+      </c>
+      <c r="J18">
+        <v>106</v>
+      </c>
+      <c r="K18">
+        <v>21</v>
+      </c>
+      <c r="L18">
+        <v>745031</v>
+      </c>
+      <c r="M18">
+        <v>759</v>
+      </c>
+      <c r="N18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>80</v>
+      </c>
+      <c r="B19">
+        <v>82</v>
+      </c>
+      <c r="C19">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>1796</v>
+      </c>
+      <c r="F19">
+        <v>858</v>
+      </c>
+      <c r="G19">
+        <v>20</v>
+      </c>
+      <c r="I19">
+        <v>239</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <v>20</v>
+      </c>
+      <c r="L19">
+        <v>116802</v>
+      </c>
+      <c r="M19">
+        <v>65</v>
+      </c>
+      <c r="N19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>85</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>7695</v>
-      </c>
-      <c r="F3">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>35</v>
-      </c>
-      <c r="B4">
-        <v>1244</v>
-      </c>
-      <c r="C4">
-        <v>65</v>
-      </c>
-      <c r="E4">
-        <v>24752</v>
-      </c>
-      <c r="F4">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>40</v>
-      </c>
-      <c r="B5">
-        <v>2924</v>
-      </c>
-      <c r="C5">
-        <v>237</v>
-      </c>
-      <c r="E5">
-        <v>7114</v>
-      </c>
-      <c r="F5">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>45</v>
-      </c>
-      <c r="B6">
-        <v>1404</v>
-      </c>
-      <c r="C6">
-        <v>89</v>
-      </c>
-      <c r="E6">
-        <v>877</v>
-      </c>
-      <c r="F6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>50</v>
-      </c>
-      <c r="B7">
-        <v>1271</v>
-      </c>
-      <c r="C7">
-        <v>71</v>
-      </c>
-      <c r="E7">
-        <v>26434</v>
-      </c>
-      <c r="F7">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>55</v>
-      </c>
-      <c r="B8">
-        <v>60</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>1635</v>
-      </c>
-      <c r="F8">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>70</v>
-      </c>
-      <c r="B9">
-        <v>3747</v>
-      </c>
-      <c r="C9">
-        <v>315</v>
-      </c>
-      <c r="E9">
-        <v>2381</v>
-      </c>
-      <c r="F9">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>75</v>
-      </c>
-      <c r="B10">
-        <v>8137</v>
-      </c>
-      <c r="C10">
-        <v>304</v>
-      </c>
-      <c r="E10">
-        <v>1829</v>
-      </c>
-      <c r="F10">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>80</v>
-      </c>
-      <c r="B11">
-        <v>2552</v>
-      </c>
-      <c r="C11">
-        <v>202</v>
-      </c>
-      <c r="E11">
-        <v>10952</v>
-      </c>
-      <c r="F11">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>85</v>
-      </c>
-      <c r="B12">
-        <v>3241</v>
-      </c>
-      <c r="C12">
-        <v>296</v>
-      </c>
-      <c r="E12">
-        <v>25299</v>
-      </c>
-      <c r="F12">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>100</v>
-      </c>
-      <c r="B13">
-        <v>2099</v>
-      </c>
-      <c r="C13">
-        <v>146</v>
-      </c>
-      <c r="E13">
-        <v>17057</v>
-      </c>
-      <c r="F13">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>120</v>
-      </c>
-      <c r="B14">
-        <v>504</v>
-      </c>
-      <c r="C14">
-        <v>22</v>
-      </c>
-      <c r="E14">
-        <v>18074</v>
-      </c>
-      <c r="F14">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>125</v>
-      </c>
-      <c r="B15">
-        <v>3284</v>
-      </c>
-      <c r="C15">
-        <v>276</v>
-      </c>
-      <c r="E15">
-        <v>23805</v>
-      </c>
-      <c r="F15">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>130</v>
-      </c>
-      <c r="B16">
-        <v>770</v>
-      </c>
-      <c r="C16">
-        <v>35</v>
-      </c>
-      <c r="E16">
-        <v>1805</v>
-      </c>
-      <c r="F16">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>150</v>
-      </c>
-      <c r="B17">
-        <v>10125</v>
-      </c>
-      <c r="C17">
-        <v>844</v>
-      </c>
-      <c r="E17">
-        <v>18830</v>
-      </c>
-      <c r="F17">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>200</v>
-      </c>
-      <c r="B18">
-        <v>3810</v>
-      </c>
-      <c r="C18">
-        <v>387</v>
-      </c>
-      <c r="E18">
-        <v>13783</v>
-      </c>
-      <c r="F18">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>250</v>
-      </c>
-      <c r="B19">
-        <v>4003</v>
-      </c>
-      <c r="C19">
-        <v>366</v>
-      </c>
-      <c r="E19">
-        <v>31562</v>
-      </c>
-      <c r="F19">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>300</v>
-      </c>
-      <c r="B20">
-        <v>4328</v>
-      </c>
-      <c r="C20">
-        <v>413</v>
+      <c r="D20">
+        <v>13</v>
       </c>
       <c r="E20">
-        <v>33661</v>
+        <v>19</v>
       </c>
       <c r="F20">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>13</v>
+      </c>
+      <c r="I20">
+        <v>27</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>13</v>
+      </c>
+      <c r="L20">
+        <v>66</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>400</v>
+        <v>90</v>
       </c>
       <c r="B21">
-        <v>2102</v>
+        <v>212</v>
       </c>
       <c r="C21">
-        <v>141</v>
+        <v>32</v>
+      </c>
+      <c r="D21">
+        <v>18</v>
       </c>
       <c r="E21">
-        <v>51394</v>
+        <v>3081</v>
       </c>
       <c r="F21">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>500</v>
-      </c>
-      <c r="B22">
-        <v>3132</v>
-      </c>
-      <c r="C22">
-        <v>252</v>
-      </c>
-      <c r="E22">
-        <v>5097</v>
-      </c>
-      <c r="F22">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>600</v>
-      </c>
-      <c r="B23">
-        <v>1093</v>
-      </c>
-      <c r="C23">
-        <v>61</v>
-      </c>
-      <c r="E23">
-        <v>26180</v>
-      </c>
-      <c r="F23">
-        <v>281</v>
+        <v>536</v>
+      </c>
+      <c r="G21">
+        <v>18</v>
+      </c>
+      <c r="I21">
+        <v>1680</v>
+      </c>
+      <c r="J21">
+        <v>27</v>
+      </c>
+      <c r="K21">
+        <v>18</v>
+      </c>
+      <c r="L21">
+        <v>1134242</v>
+      </c>
+      <c r="M21">
+        <v>6</v>
+      </c>
+      <c r="N21">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
+  <mergeCells count="6">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>